<commit_message>
Revisions to specimen ID and PCoA axis titles
</commit_message>
<xml_diff>
--- a/data/raw/guadua_lemmas_paleas_raw_3.xlsx
+++ b/data/raw/guadua_lemmas_paleas_raw_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkam\Documents\Guadua_leaf_project\guadua_leaf\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291E5250-A0E3-4067-B43E-7BD0699F05B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C297F9-6C92-4D08-AD67-9D19415BED9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6465" yWindow="2430" windowWidth="21615" windowHeight="11325" xr2:uid="{4A5E8B54-E7AB-40A1-88CA-D7612C0FD733}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A5E8B54-E7AB-40A1-88CA-D7612C0FD733}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -603,9 +603,6 @@
     <t>G_trinii_Hatschbach_and_Cervi_53238</t>
   </si>
   <si>
-    <t>Unknown_G_aff_weberbaueri_Renvoize_4671</t>
-  </si>
-  <si>
     <t>general_habitat</t>
   </si>
   <si>
@@ -720,16 +717,19 @@
     <t>G_aff_weberbaueri</t>
   </si>
   <si>
-    <t>Unknown_G_aff_sarcocarpa_Calderon_2282</t>
-  </si>
-  <si>
     <t>G_refracta_Hatschbach_and_Cervi_52445</t>
   </si>
   <si>
     <t>G_refracta</t>
   </si>
   <si>
-    <t>G_aff_sarcocarpa</t>
+    <t>Undescribed_G_aff_glomerata_Calderon_2282</t>
+  </si>
+  <si>
+    <t>G_aff_glomerata</t>
+  </si>
+  <si>
+    <t>Undescribed_G_aff_weberbaueri_Renvoize_4671</t>
   </si>
 </sst>
 </file>
@@ -1127,8 +1127,8 @@
   <dimension ref="A1:BA93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,7 +1190,7 @@
         <v>179</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>178</v>
@@ -1205,13 +1205,13 @@
         <v>182</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>144</v>
@@ -1265,13 +1265,13 @@
         <v>158</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AG1" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AH1" s="4" t="s">
         <v>159</v>
@@ -1351,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
@@ -1512,7 +1512,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>5</v>
@@ -1673,7 +1673,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>5</v>
@@ -1834,7 +1834,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>5</v>
@@ -1995,7 +1995,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>5</v>
@@ -2156,7 +2156,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>5</v>
@@ -2317,7 +2317,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>5</v>
@@ -2478,7 +2478,7 @@
         <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>5</v>
@@ -2639,7 +2639,7 @@
         <v>13</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>5</v>
@@ -2800,7 +2800,7 @@
         <v>13</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>5</v>
@@ -2961,7 +2961,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>5</v>
@@ -3122,7 +3122,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>5</v>
@@ -3283,7 +3283,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>5</v>
@@ -3444,7 +3444,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>5</v>
@@ -3605,7 +3605,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>33</v>
@@ -3766,7 +3766,7 @@
         <v>4</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>33</v>
@@ -3927,7 +3927,7 @@
         <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>5</v>
@@ -4088,7 +4088,7 @@
         <v>13</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>5</v>
@@ -4234,7 +4234,7 @@
     </row>
     <row r="20" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -4249,7 +4249,7 @@
         <v>13</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>5</v>
@@ -4395,13 +4395,13 @@
     </row>
     <row r="21" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
@@ -4410,7 +4410,7 @@
         <v>13</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>5</v>
@@ -4556,7 +4556,7 @@
     </row>
     <row r="22" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>94</v>
@@ -4571,7 +4571,7 @@
         <v>13</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>33</v>
@@ -4732,7 +4732,7 @@
         <v>13</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>33</v>
@@ -4893,7 +4893,7 @@
         <v>13</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>33</v>
@@ -5054,7 +5054,7 @@
         <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>33</v>
@@ -5200,7 +5200,7 @@
     </row>
     <row r="26" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>94</v>
@@ -5215,7 +5215,7 @@
         <v>13</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>33</v>
@@ -5361,7 +5361,7 @@
     </row>
     <row r="27" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>105</v>
@@ -5376,7 +5376,7 @@
         <v>13</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>33</v>
@@ -5522,7 +5522,7 @@
     </row>
     <row r="28" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>105</v>
@@ -5537,7 +5537,7 @@
         <v>13</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>33</v>
@@ -5683,7 +5683,7 @@
     </row>
     <row r="29" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>105</v>
@@ -5698,7 +5698,7 @@
         <v>13</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>33</v>
@@ -5859,7 +5859,7 @@
         <v>4</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>5</v>
@@ -6020,7 +6020,7 @@
         <v>13</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>5</v>
@@ -6181,7 +6181,7 @@
         <v>13</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>5</v>
@@ -6327,7 +6327,7 @@
     </row>
     <row r="33" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
@@ -6342,7 +6342,7 @@
         <v>13</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>5</v>
@@ -6503,7 +6503,7 @@
         <v>13</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>5</v>
@@ -6664,7 +6664,7 @@
         <v>13</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>17</v>
@@ -6810,13 +6810,13 @@
     </row>
     <row r="36" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>20</v>
@@ -6825,7 +6825,7 @@
         <v>13</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>17</v>
@@ -6986,7 +6986,7 @@
         <v>13</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>17</v>
@@ -7147,7 +7147,7 @@
         <v>4</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>17</v>
@@ -7293,7 +7293,7 @@
     </row>
     <row r="39" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>46</v>
@@ -7308,7 +7308,7 @@
         <v>13</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>33</v>
@@ -7469,7 +7469,7 @@
         <v>13</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>33</v>
@@ -7630,7 +7630,7 @@
         <v>13</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>33</v>
@@ -7776,7 +7776,7 @@
     </row>
     <row r="42" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>46</v>
@@ -7791,7 +7791,7 @@
         <v>13</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>33</v>
@@ -7937,7 +7937,7 @@
     </row>
     <row r="43" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>46</v>
@@ -7952,7 +7952,7 @@
         <v>13</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>33</v>
@@ -8098,7 +8098,7 @@
     </row>
     <row r="44" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>47</v>
@@ -8113,7 +8113,7 @@
         <v>4</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>5</v>
@@ -8259,7 +8259,7 @@
     </row>
     <row r="45" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>47</v>
@@ -8274,7 +8274,7 @@
         <v>4</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>5</v>
@@ -8435,7 +8435,7 @@
         <v>4</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>5</v>
@@ -8596,7 +8596,7 @@
         <v>4</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>5</v>
@@ -9723,7 +9723,7 @@
         <v>4</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>5</v>
@@ -9869,13 +9869,13 @@
     </row>
     <row r="55" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>8</v>
@@ -9884,7 +9884,7 @@
         <v>4</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>5</v>
@@ -10030,10 +10030,10 @@
     </row>
     <row r="56" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>23</v>
@@ -10191,7 +10191,7 @@
     </row>
     <row r="57" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>51</v>
@@ -10206,7 +10206,7 @@
         <v>4</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>33</v>
@@ -10352,7 +10352,7 @@
     </row>
     <row r="58" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>51</v>
@@ -10367,7 +10367,7 @@
         <v>4</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>33</v>
@@ -10528,7 +10528,7 @@
         <v>13</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>5</v>
@@ -10689,7 +10689,7 @@
         <v>13</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>5</v>
@@ -10850,7 +10850,7 @@
         <v>13</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>5</v>
@@ -11011,7 +11011,7 @@
         <v>13</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>5</v>
@@ -11172,7 +11172,7 @@
         <v>4</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>33</v>
@@ -11318,7 +11318,7 @@
     </row>
     <row r="64" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>29</v>
@@ -11333,7 +11333,7 @@
         <v>4</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>33</v>
@@ -11494,7 +11494,7 @@
         <v>4</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>33</v>
@@ -11640,7 +11640,7 @@
     </row>
     <row r="66" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>29</v>
@@ -11655,7 +11655,7 @@
         <v>4</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>33</v>
@@ -11816,7 +11816,7 @@
         <v>4</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>17</v>
@@ -11977,7 +11977,7 @@
         <v>4</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>17</v>
@@ -12138,7 +12138,7 @@
         <v>4</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>17</v>
@@ -12299,7 +12299,7 @@
         <v>4</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>17</v>
@@ -12460,7 +12460,7 @@
         <v>4</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>17</v>
@@ -12621,7 +12621,7 @@
         <v>4</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>5</v>
@@ -12782,7 +12782,7 @@
         <v>13</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>5</v>
@@ -12928,7 +12928,7 @@
     </row>
     <row r="74" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>50</v>
@@ -12943,7 +12943,7 @@
         <v>13</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>5</v>
@@ -13089,7 +13089,7 @@
     </row>
     <row r="75" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>124</v>
@@ -13572,7 +13572,7 @@
     </row>
     <row r="78" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>124</v>
@@ -13733,7 +13733,7 @@
     </row>
     <row r="79" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>124</v>
@@ -13894,7 +13894,7 @@
     </row>
     <row r="80" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>124</v>
@@ -14070,7 +14070,7 @@
         <v>4</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>33</v>
@@ -14231,7 +14231,7 @@
         <v>4</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>33</v>
@@ -14377,7 +14377,7 @@
     </row>
     <row r="83" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>31</v>
@@ -14392,7 +14392,7 @@
         <v>4</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>33</v>
@@ -14538,7 +14538,7 @@
     </row>
     <row r="84" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>31</v>
@@ -14553,7 +14553,7 @@
         <v>4</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>33</v>
@@ -14699,7 +14699,7 @@
     </row>
     <row r="85" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>31</v>
@@ -14714,7 +14714,7 @@
         <v>4</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>33</v>
@@ -14875,7 +14875,7 @@
         <v>4</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>33</v>
@@ -15021,10 +15021,10 @@
     </row>
     <row r="87" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>23</v>
@@ -15036,7 +15036,7 @@
         <v>4</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>33</v>
@@ -15182,10 +15182,10 @@
     </row>
     <row r="88" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>192</v>
+        <v>234</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>7</v>
@@ -15197,7 +15197,7 @@
         <v>13</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>33</v>

</xml_diff>